<commit_message>
Lesson 16 - Database  - 16.02.2024
</commit_message>
<xml_diff>
--- a/Java23 VoAnhTuan Database Design.xlsx
+++ b/Java23 VoAnhTuan Database Design.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - plan and doc\Phần 3 - Database(MySQL)\16. RBDMS\DEMO\RDBMS demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoc Lap Trinh web\java23\3.Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7B2B7C-989C-4DF6-9A8C-2B9CEB10207E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB7D385-5CC6-49E6-813F-A07024975B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="588" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" tabRatio="588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mô hình quan niệm" sheetId="1" r:id="rId1"/>
-    <sheet name="ERD - Mô hình logic" sheetId="2" r:id="rId2"/>
-    <sheet name="RD - Mô hình quan hệ" sheetId="3" r:id="rId3"/>
-    <sheet name="DB - Mô hình vật lý" sheetId="4" r:id="rId4"/>
+    <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
+    <sheet name="B2. Mô hình logic" sheetId="5" r:id="rId2"/>
+    <sheet name="ERD - Mô hình logic" sheetId="2" r:id="rId3"/>
+    <sheet name="RD - Mô hình quan hệ" sheetId="3" r:id="rId4"/>
+    <sheet name="DB - Mô hình vật lý" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="266">
   <si>
     <t>MatHang</t>
   </si>
@@ -837,12 +838,123 @@
   <si>
     <t>Trigger, View</t>
   </si>
+  <si>
+    <t>LoaiHang</t>
+  </si>
+  <si>
+    <t>ChucVu</t>
+  </si>
+  <si>
+    <t>ThongTinNhapHang</t>
+  </si>
+  <si>
+    <t>PhuongThucThanhToan</t>
+  </si>
+  <si>
+    <t>TrangThaiDonHang</t>
+  </si>
+  <si>
+    <t>KichCo(s)</t>
+  </si>
+  <si>
+    <t>ChatLieu(s)</t>
+  </si>
+  <si>
+    <t>MauSac(s)</t>
+  </si>
+  <si>
+    <t>HinhAnh(s)</t>
+  </si>
+  <si>
+    <t>TenLH</t>
+  </si>
+  <si>
+    <t>DiaChiGiaoHang</t>
+  </si>
+  <si>
+    <t>NguoiTao</t>
+  </si>
+  <si>
+    <t>TongTien</t>
+  </si>
+  <si>
+    <t>TenNV</t>
+  </si>
+  <si>
+    <t>SoDienThoai</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>GioiTinh</t>
+  </si>
+  <si>
+    <t>NgaySinh</t>
+  </si>
+  <si>
+    <t>MatKhau</t>
+  </si>
+  <si>
+    <t>MaNV</t>
+  </si>
+  <si>
+    <t>TaiKhoan</t>
+  </si>
+  <si>
+    <t>MaTK</t>
+  </si>
+  <si>
+    <t>TenTK</t>
+  </si>
+  <si>
+    <t>TrangThai</t>
+  </si>
+  <si>
+    <t>MaCV</t>
+  </si>
+  <si>
+    <t>TenCV</t>
+  </si>
+  <si>
+    <t>MaPN</t>
+  </si>
+  <si>
+    <t>SoLuongNhap</t>
+  </si>
+  <si>
+    <t>GiaNhap</t>
+  </si>
+  <si>
+    <t>NgayNhapHang</t>
+  </si>
+  <si>
+    <t>NhaCungCap</t>
+  </si>
+  <si>
+    <t>MaPTTT</t>
+  </si>
+  <si>
+    <t>TenPTTT</t>
+  </si>
+  <si>
+    <t>TinhTrangDon</t>
+  </si>
+  <si>
+    <t>NhanVienPhuTrach</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/12g4aTrsdVaLsj6B9soJ1t-MSPUay6PJd/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Link Drive:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -928,6 +1040,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1045,10 +1172,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1205,8 +1333,24 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1534,133 +1678,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:K24"/>
+  <dimension ref="B4:L24"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="73" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="20" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+    <col min="13" max="21" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="D8" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>252</v>
+      </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="60" t="s">
+        <v>229</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>245</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>258</v>
+      </c>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="60" t="s">
+        <v>235</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="60" t="s">
+        <v>232</v>
+      </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>246</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="60" t="s">
+        <v>240</v>
+      </c>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="60" t="s">
+        <v>236</v>
+      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="60" t="s">
+        <v>240</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" s="60" t="s">
+        <v>230</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>259</v>
+      </c>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="60" t="s">
+        <v>237</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="60" t="s">
+        <v>249</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1670,8 +1955,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1682,8 +1968,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1694,8 +1981,9 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1706,8 +1994,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1718,8 +2007,9 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1730,8 +2020,9 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1742,8 +2033,9 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1754,39 +2046,487 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="19" t="s">
         <v>110</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="24" spans="2:11" s="18" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:12" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65EF1A4-4C62-4B5F-86C4-AC4D70F77F2E}">
+  <dimension ref="A4:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+    <col min="13" max="21" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="H5" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" s="63" t="s">
+        <v>253</v>
+      </c>
+      <c r="J5" s="63" t="s">
+        <v>255</v>
+      </c>
+      <c r="K5" s="63" t="s">
+        <v>260</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="60" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="60" t="s">
+        <v>240</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="60" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="60" t="s">
+        <v>240</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+    </row>
+    <row r="24" spans="1:12" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="61"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="61"/>
+      <c r="C27" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="66" t="s">
+        <v>265</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" xr:uid="{AF7E4E43-4050-4E3D-BE7A-6BE86763297B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:U43"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScale="73" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>112</v>
       </c>
@@ -1799,7 +2539,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1807,7 +2547,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1816,10 +2556,10 @@
       </c>
       <c r="P4" s="52"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N5" s="52"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>43</v>
       </c>
@@ -1831,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D8" s="5"/>
       <c r="P8" s="25" t="s">
         <v>59</v>
@@ -1840,7 +2580,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
@@ -1881,7 +2621,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>45</v>
       </c>
@@ -1922,7 +2662,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>63</v>
       </c>
@@ -1957,7 +2697,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>46</v>
       </c>
@@ -1992,7 +2732,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>57</v>
       </c>
@@ -2015,7 +2755,7 @@
       <c r="T13" s="54"/>
       <c r="U13" s="54"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D14" s="5"/>
       <c r="O14" s="13" t="s">
         <v>43</v>
@@ -2031,15 +2771,15 @@
       <c r="T14" s="54"/>
       <c r="U14" s="54"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J16" s="52"/>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>37</v>
       </c>
@@ -2059,7 +2799,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -2070,7 +2810,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
@@ -2099,7 +2839,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="12">
         <v>1</v>
       </c>
@@ -2122,7 +2862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>54</v>
       </c>
@@ -2154,7 +2894,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>3</v>
       </c>
@@ -2181,7 +2921,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G23" s="5">
         <v>4</v>
       </c>
@@ -2198,7 +2938,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G24" s="5">
         <v>5</v>
       </c>
@@ -2212,7 +2952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G25" s="5">
         <v>6</v>
       </c>
@@ -2226,7 +2966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G26" s="5">
         <v>7</v>
       </c>
@@ -2240,12 +2980,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>70</v>
       </c>
@@ -2256,12 +2996,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
         <v>72</v>
       </c>
@@ -2270,7 +3010,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
         <v>73</v>
       </c>
@@ -2282,40 +3022,40 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I36" s="49"/>
       <c r="J36" s="49"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I37" s="49"/>
       <c r="J37" s="49"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I38" s="49"/>
       <c r="J38" s="49"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I39" s="49"/>
       <c r="J39" s="49"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I40" s="49"/>
       <c r="J40" s="49"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I41" s="49"/>
       <c r="J41" s="49"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I42" s="53"/>
       <c r="J42" s="53"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I43" s="49"/>
       <c r="J43" s="49"/>
     </row>
@@ -2328,23 +3068,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AJ77"/>
   <sheetViews>
-    <sheetView topLeftCell="S34" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="P30" zoomScale="122" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="Y48" sqref="Y48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="8.85546875" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="33" max="33" width="17.7109375" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" customWidth="1"/>
     <col min="34" max="34" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -2352,12 +3092,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>79</v>
       </c>
@@ -2369,7 +3109,7 @@
       </c>
       <c r="U4" s="20"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>80</v>
       </c>
@@ -2401,7 +3141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>81</v>
       </c>
@@ -2427,7 +3167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -2453,7 +3193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -2479,7 +3219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -2496,7 +3236,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C10" s="23" t="s">
         <v>209</v>
       </c>
@@ -2526,7 +3266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>210</v>
       </c>
@@ -2550,7 +3290,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="P12" s="4" t="s">
         <v>67</v>
       </c>
@@ -2559,7 +3299,7 @@
       </c>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="P13" s="4" t="s">
         <v>85</v>
       </c>
@@ -2571,7 +3311,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="P14" s="4" t="s">
         <v>86</v>
       </c>
@@ -2583,12 +3323,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="T15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
@@ -2600,7 +3340,7 @@
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
     </row>
-    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:35" x14ac:dyDescent="0.3">
       <c r="T18" s="22" t="s">
         <v>103</v>
       </c>
@@ -2608,7 +3348,7 @@
       <c r="V18" s="21"/>
       <c r="W18" s="5"/>
     </row>
-    <row r="19" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:35" x14ac:dyDescent="0.3">
       <c r="P19" s="59" t="s">
         <v>11</v>
       </c>
@@ -2626,7 +3366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:35" x14ac:dyDescent="0.3">
       <c r="P20" s="4" t="s">
         <v>12</v>
       </c>
@@ -2647,7 +3387,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:35" x14ac:dyDescent="0.3">
       <c r="P21" s="4">
         <v>1</v>
       </c>
@@ -2668,7 +3408,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:35" x14ac:dyDescent="0.3">
       <c r="P22" s="4">
         <v>2</v>
       </c>
@@ -2689,7 +3429,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:35" x14ac:dyDescent="0.3">
       <c r="P23" s="4">
         <v>3</v>
       </c>
@@ -2711,7 +3451,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:35" x14ac:dyDescent="0.3">
       <c r="P24" s="4">
         <v>4</v>
       </c>
@@ -2738,7 +3478,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:35" x14ac:dyDescent="0.3">
       <c r="T28" s="22" t="s">
         <v>156</v>
       </c>
@@ -2757,7 +3497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C29" s="21" t="s">
         <v>122</v>
       </c>
@@ -2813,7 +3553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C30" s="6" t="s">
         <v>123</v>
       </c>
@@ -2889,7 +3629,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C31" s="48" t="s">
         <v>126</v>
       </c>
@@ -2965,7 +3705,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C32" s="48" t="s">
         <v>127</v>
       </c>
@@ -3036,7 +3776,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="33" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C33" s="48" t="s">
         <v>128</v>
       </c>
@@ -3101,7 +3841,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C34" s="48" t="s">
         <v>144</v>
       </c>
@@ -3133,7 +3873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C35" s="48" t="s">
         <v>148</v>
       </c>
@@ -3156,7 +3896,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="37" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C37" s="34" t="s">
         <v>152</v>
       </c>
@@ -3191,7 +3931,7 @@
       <c r="AI37" s="9"/>
       <c r="AJ37" s="9"/>
     </row>
-    <row r="38" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>138</v>
       </c>
@@ -3202,7 +3942,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>139</v>
       </c>
@@ -3213,7 +3953,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>218</v>
       </c>
@@ -3224,7 +3964,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>137</v>
       </c>
@@ -3232,7 +3972,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>140</v>
       </c>
@@ -3247,12 +3987,12 @@
       <c r="AG42" s="46"/>
       <c r="AH42" s="46"/>
     </row>
-    <row r="43" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
         <v>146</v>
       </c>
@@ -3266,7 +4006,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="45" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
         <v>142</v>
       </c>
@@ -3295,7 +4035,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
         <v>143</v>
       </c>
@@ -3330,7 +4070,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
         <v>219</v>
       </c>
@@ -3362,7 +4102,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="3:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C48" s="55" t="s">
         <v>221</v>
       </c>
@@ -3401,7 +4141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="3:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="57" t="s">
         <v>220</v>
       </c>
@@ -3440,7 +4180,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:32" x14ac:dyDescent="0.3">
       <c r="O50" s="29">
         <v>5</v>
       </c>
@@ -3460,7 +4200,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:32" x14ac:dyDescent="0.3">
       <c r="O51" s="29">
         <v>6</v>
       </c>
@@ -3480,7 +4220,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C52" s="21" t="s">
         <v>122</v>
       </c>
@@ -3506,7 +4246,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="53" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C53" s="6" t="s">
         <v>123</v>
       </c>
@@ -3541,7 +4281,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C54" s="48" t="s">
         <v>126</v>
       </c>
@@ -3569,7 +4309,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C55" s="48" t="s">
         <v>127</v>
       </c>
@@ -3607,7 +4347,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C56" s="48" t="s">
         <v>128</v>
       </c>
@@ -3642,7 +4382,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C57" s="48" t="s">
         <v>144</v>
       </c>
@@ -3668,7 +4408,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C58" s="48" t="s">
         <v>148</v>
       </c>
@@ -3694,7 +4434,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="59" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:32" x14ac:dyDescent="0.3">
       <c r="O59" s="29">
         <v>14</v>
       </c>
@@ -3708,7 +4448,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="60" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:32" x14ac:dyDescent="0.3">
       <c r="O60" s="29">
         <v>15</v>
       </c>
@@ -3722,7 +4462,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:32" x14ac:dyDescent="0.3">
       <c r="O61" s="29">
         <v>16</v>
       </c>
@@ -3736,7 +4476,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="17:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="17:24" x14ac:dyDescent="0.3">
       <c r="Q71" s="21" t="s">
         <v>122</v>
       </c>
@@ -3745,7 +4485,7 @@
       </c>
       <c r="X71" s="22"/>
     </row>
-    <row r="72" spans="17:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="17:24" x14ac:dyDescent="0.3">
       <c r="Q72" s="6" t="s">
         <v>123</v>
       </c>
@@ -3765,7 +4505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="17:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="17:24" x14ac:dyDescent="0.3">
       <c r="Q73" s="4" t="s">
         <v>126</v>
       </c>
@@ -3785,7 +4525,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="17:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="17:24" x14ac:dyDescent="0.3">
       <c r="Q74" s="4" t="s">
         <v>127</v>
       </c>
@@ -3805,7 +4545,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="17:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="17:24" x14ac:dyDescent="0.3">
       <c r="Q75" s="4" t="s">
         <v>128</v>
       </c>
@@ -3825,7 +4565,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="17:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="17:24" x14ac:dyDescent="0.3">
       <c r="Q76" s="4" t="s">
         <v>144</v>
       </c>
@@ -3839,7 +4579,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="17:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="17:24" x14ac:dyDescent="0.3">
       <c r="Q77" s="4" t="s">
         <v>148</v>
       </c>
@@ -3866,35 +4606,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="121" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="7" width="21.140625" customWidth="1"/>
+    <col min="1" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="7" width="21.109375" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="22" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="15" max="22" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>78</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="4" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3909,7 +4649,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -3924,7 +4664,7 @@
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
     </row>
-    <row r="6" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="17"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3939,7 +4679,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
@@ -3954,7 +4694,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="16"/>
@@ -3969,7 +4709,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
@@ -3984,7 +4724,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
@@ -3999,7 +4739,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
@@ -4014,7 +4754,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -4029,7 +4769,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
@@ -4044,7 +4784,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
@@ -4059,7 +4799,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -4074,7 +4814,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -4089,7 +4829,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
@@ -4104,7 +4844,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
@@ -4119,7 +4859,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
@@ -4134,7 +4874,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
@@ -4149,22 +4889,22 @@
       <c r="M20" s="2"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>109</v>
       </c>

</xml_diff>